<commit_message>
use fieldlabelbuilder for complex types
</commit_message>
<xml_diff>
--- a/src/test/resources/containerMultipleChildren.xlsx
+++ b/src/test/resources/containerMultipleChildren.xlsx
@@ -25,13 +25,13 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">child1 Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">child2 Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anotherRelation Length</t>
+    <t xml:space="preserve">Child1 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child2 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnotherRelation Length</t>
   </si>
   <si>
     <t xml:space="preserve">main</t>
@@ -57,6 +57,7 @@
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,7 +152,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>